<commit_message>
next is ball type
</commit_message>
<xml_diff>
--- a/Assets/2048.xlsx
+++ b/Assets/2048.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="17940" activeTab="6"/>
+    <workbookView windowWidth="14610" windowHeight="17430" firstSheet="2" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="球颜色、大小" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="38">
   <si>
     <t>数字</t>
   </si>
@@ -109,24 +109,6 @@
     <t>金额（个位数取0）</t>
   </si>
   <si>
-    <t>1~3</t>
-  </si>
-  <si>
-    <t>200~250</t>
-  </si>
-  <si>
-    <t>3~10</t>
-  </si>
-  <si>
-    <t>150~200</t>
-  </si>
-  <si>
-    <t>&gt;=10</t>
-  </si>
-  <si>
-    <t>50~100</t>
-  </si>
-  <si>
     <t>惊喜礼盒</t>
   </si>
   <si>
@@ -153,21 +135,18 @@
   <si>
     <t>金币（个位取0）</t>
   </si>
-  <si>
-    <t>150~250</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="6">
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="176" formatCode="#,##0.00_ "/>
     <numFmt numFmtId="177" formatCode="0.000_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="24">
     <font>
@@ -209,9 +188,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FF006100"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -221,6 +199,14 @@
       <color theme="0"/>
       <name val="宋体"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -238,47 +224,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FF3F3F3F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -307,11 +255,34 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -338,11 +309,19 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="宋体"/>
-      <charset val="134"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -355,7 +334,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -367,7 +346,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -379,19 +358,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -409,55 +406,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -469,49 +436,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -529,18 +460,66 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="24">
+  <borders count="32">
     <border>
       <left/>
       <right/>
@@ -552,12 +531,84 @@
       <left style="medium">
         <color auto="1"/>
       </left>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
       <right style="medium">
         <color auto="1"/>
       </right>
       <top style="medium">
         <color auto="1"/>
       </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
       <bottom style="medium">
         <color auto="1"/>
       </bottom>
@@ -579,6 +630,32 @@
       <diagonal/>
     </border>
     <border>
+      <left style="medium">
+        <color rgb="FF999999"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color rgb="FF999999"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF999999"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FF999999"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF999999"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF999999"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right style="thick">
         <color auto="1"/>
@@ -718,6 +795,39 @@
       <top/>
       <bottom style="thin">
         <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -737,15 +847,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -757,6 +858,17 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -780,42 +892,7 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -827,10 +904,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="15" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="20" borderId="28" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -839,198 +916,228 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="25" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="24" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="24" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="31" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="27" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="28" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="24" borderId="30" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="26" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="29" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="32" borderId="23" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="22" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="18" borderId="19" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="21" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1042,22 +1149,22 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1431,169 +1538,169 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="40" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="30" t="s">
+      <c r="B1" s="40" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="30" t="s">
+      <c r="C1" s="40" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:12">
-      <c r="A2" s="30">
+      <c r="A2" s="40">
         <v>2</v>
       </c>
-      <c r="B2" s="31">
+      <c r="B2" s="41">
         <v>0.357</v>
       </c>
-      <c r="C2" s="30">
-        <v>10</v>
-      </c>
-      <c r="E2" s="32"/>
-      <c r="G2" s="31"/>
-      <c r="L2" s="32"/>
+      <c r="C2" s="40">
+        <v>10</v>
+      </c>
+      <c r="E2" s="42"/>
+      <c r="G2" s="41"/>
+      <c r="L2" s="42"/>
     </row>
     <row r="3" spans="1:12">
-      <c r="A3" s="30">
+      <c r="A3" s="40">
         <v>4</v>
       </c>
-      <c r="B3" s="31">
+      <c r="B3" s="41">
         <v>0.432727272727273</v>
       </c>
-      <c r="C3" s="30">
+      <c r="C3" s="40">
         <v>14</v>
       </c>
-      <c r="E3" s="32"/>
-      <c r="G3" s="31"/>
-      <c r="L3" s="32"/>
+      <c r="E3" s="42"/>
+      <c r="G3" s="41"/>
+      <c r="L3" s="42"/>
     </row>
     <row r="4" spans="1:12">
-      <c r="A4" s="30">
+      <c r="A4" s="40">
         <v>8</v>
       </c>
-      <c r="B4" s="31">
+      <c r="B4" s="41">
         <v>0.519272727272727</v>
       </c>
-      <c r="C4" s="30">
+      <c r="C4" s="40">
         <v>5</v>
       </c>
-      <c r="E4" s="32"/>
-      <c r="G4" s="31"/>
-      <c r="L4" s="32"/>
+      <c r="E4" s="42"/>
+      <c r="G4" s="41"/>
+      <c r="L4" s="42"/>
     </row>
     <row r="5" spans="1:12">
-      <c r="A5" s="30">
+      <c r="A5" s="40">
         <v>16</v>
       </c>
-      <c r="B5" s="31">
+      <c r="B5" s="41">
         <v>0.616636363636363</v>
       </c>
-      <c r="C5" s="30">
-        <v>6</v>
-      </c>
-      <c r="E5" s="32"/>
-      <c r="G5" s="31"/>
-      <c r="L5" s="32"/>
+      <c r="C5" s="40">
+        <v>6</v>
+      </c>
+      <c r="E5" s="42"/>
+      <c r="G5" s="41"/>
+      <c r="L5" s="42"/>
     </row>
     <row r="6" spans="1:12">
-      <c r="A6" s="30">
+      <c r="A6" s="40">
         <v>32</v>
       </c>
-      <c r="B6" s="31">
+      <c r="B6" s="41">
         <v>0.649090909090907</v>
       </c>
-      <c r="C6" s="30">
+      <c r="C6" s="40">
         <v>3</v>
       </c>
-      <c r="E6" s="32"/>
-      <c r="G6" s="31"/>
-      <c r="L6" s="32"/>
+      <c r="E6" s="42"/>
+      <c r="G6" s="41"/>
+      <c r="L6" s="42"/>
     </row>
     <row r="7" spans="1:12">
-      <c r="A7" s="30">
+      <c r="A7" s="40">
         <v>64</v>
       </c>
-      <c r="B7" s="31">
+      <c r="B7" s="41">
         <v>0.811363636363632</v>
       </c>
-      <c r="C7" s="30">
+      <c r="C7" s="40">
         <v>7</v>
       </c>
-      <c r="E7" s="32"/>
-      <c r="G7" s="31"/>
-      <c r="L7" s="32"/>
+      <c r="E7" s="42"/>
+      <c r="G7" s="41"/>
+      <c r="L7" s="42"/>
     </row>
     <row r="8" spans="1:12">
-      <c r="A8" s="30">
+      <c r="A8" s="40">
         <v>128</v>
       </c>
-      <c r="B8" s="31">
+      <c r="B8" s="41">
         <v>0.887090909090904</v>
       </c>
-      <c r="C8" s="30">
+      <c r="C8" s="40">
         <v>8</v>
       </c>
-      <c r="E8" s="32"/>
-      <c r="G8" s="31"/>
-      <c r="L8" s="32"/>
+      <c r="E8" s="42"/>
+      <c r="G8" s="41"/>
+      <c r="L8" s="42"/>
     </row>
     <row r="9" spans="1:12">
-      <c r="A9" s="30">
+      <c r="A9" s="40">
         <v>256</v>
       </c>
-      <c r="B9" s="31">
+      <c r="B9" s="41">
         <v>0.973636363636364</v>
       </c>
-      <c r="C9" s="30">
+      <c r="C9" s="40">
         <v>15</v>
       </c>
-      <c r="E9" s="32"/>
-      <c r="G9" s="31"/>
-      <c r="L9" s="32"/>
+      <c r="E9" s="42"/>
+      <c r="G9" s="41"/>
+      <c r="L9" s="42"/>
     </row>
     <row r="10" spans="1:12">
-      <c r="A10" s="30">
+      <c r="A10" s="40">
         <v>512</v>
       </c>
-      <c r="B10" s="31">
+      <c r="B10" s="41">
         <v>1.04936363636364</v>
       </c>
-      <c r="C10" s="30">
+      <c r="C10" s="40">
         <v>11</v>
       </c>
-      <c r="E10" s="32"/>
-      <c r="G10" s="31"/>
-      <c r="L10" s="32"/>
+      <c r="E10" s="42"/>
+      <c r="G10" s="41"/>
+      <c r="L10" s="42"/>
     </row>
     <row r="11" spans="1:12">
-      <c r="A11" s="30">
+      <c r="A11" s="40">
         <v>1024</v>
       </c>
-      <c r="B11" s="31">
+      <c r="B11" s="41">
         <v>1.19</v>
       </c>
-      <c r="C11" s="30">
+      <c r="C11" s="40">
         <v>13</v>
       </c>
-      <c r="E11" s="32"/>
-      <c r="G11" s="31"/>
-      <c r="L11" s="32"/>
+      <c r="E11" s="42"/>
+      <c r="G11" s="41"/>
+      <c r="L11" s="42"/>
     </row>
     <row r="12" spans="1:12">
-      <c r="A12" s="30">
+      <c r="A12" s="40">
         <v>2048</v>
       </c>
-      <c r="B12" s="31">
+      <c r="B12" s="41">
         <v>1.42259090909091</v>
       </c>
-      <c r="C12" s="30">
+      <c r="C12" s="40">
         <v>16</v>
       </c>
-      <c r="E12" s="32"/>
-      <c r="G12" s="31"/>
-      <c r="L12" s="32"/>
+      <c r="E12" s="42"/>
+      <c r="G12" s="41"/>
+      <c r="L12" s="42"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1618,270 +1725,270 @@
   </cols>
   <sheetData>
     <row r="1" ht="16.5" spans="1:9">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18" t="s">
+      <c r="B1" s="28"/>
+      <c r="C1" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
-      <c r="I1" s="27"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="28"/>
+      <c r="I1" s="37"/>
     </row>
     <row r="2" ht="16.5" spans="1:9">
-      <c r="A2" s="19"/>
-      <c r="B2" s="14"/>
-      <c r="C2" s="14">
+      <c r="A2" s="29"/>
+      <c r="B2" s="24"/>
+      <c r="C2" s="24">
         <v>2</v>
       </c>
-      <c r="D2" s="14">
+      <c r="D2" s="24">
         <v>4</v>
       </c>
-      <c r="E2" s="14">
+      <c r="E2" s="24">
         <v>8</v>
       </c>
-      <c r="F2" s="14">
+      <c r="F2" s="24">
         <v>16</v>
       </c>
-      <c r="G2" s="14">
+      <c r="G2" s="24">
         <v>32</v>
       </c>
-      <c r="H2" s="14">
+      <c r="H2" s="24">
         <v>64</v>
       </c>
-      <c r="I2" s="28">
+      <c r="I2" s="38">
         <v>128</v>
       </c>
     </row>
     <row r="3" ht="16.5" spans="1:9">
-      <c r="A3" s="19"/>
-      <c r="B3" s="14"/>
-      <c r="C3" s="14" t="s">
+      <c r="A3" s="29"/>
+      <c r="B3" s="24"/>
+      <c r="C3" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="14" t="s">
+      <c r="D3" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="14" t="s">
+      <c r="E3" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="14" t="s">
+      <c r="F3" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="14" t="s">
+      <c r="G3" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="H3" s="14" t="s">
+      <c r="H3" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="I3" s="28" t="s">
+      <c r="I3" s="38" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="4" ht="16.5" spans="1:9">
-      <c r="A4" s="20" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="21">
+      <c r="A4" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="31">
         <v>128</v>
       </c>
-      <c r="C4" s="14">
+      <c r="C4" s="24">
         <v>100</v>
       </c>
-      <c r="D4" s="14">
+      <c r="D4" s="24">
         <v>100</v>
       </c>
-      <c r="E4" s="14">
+      <c r="E4" s="24">
         <v>80</v>
       </c>
-      <c r="F4" s="14">
+      <c r="F4" s="24">
         <v>20</v>
       </c>
-      <c r="G4" s="14">
+      <c r="G4" s="24">
         <v>0</v>
       </c>
-      <c r="H4" s="14">
+      <c r="H4" s="24">
         <v>0</v>
       </c>
-      <c r="I4" s="28">
+      <c r="I4" s="38">
         <v>0</v>
       </c>
     </row>
     <row r="5" ht="16.5" spans="1:9">
-      <c r="A5" s="20" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="21">
+      <c r="A5" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="31">
         <v>256</v>
       </c>
-      <c r="C5" s="14">
+      <c r="C5" s="24">
         <v>80</v>
       </c>
-      <c r="D5" s="14">
+      <c r="D5" s="24">
         <v>90</v>
       </c>
-      <c r="E5" s="14">
+      <c r="E5" s="24">
         <v>80</v>
       </c>
-      <c r="F5" s="14">
+      <c r="F5" s="24">
         <v>50</v>
       </c>
-      <c r="G5" s="14">
+      <c r="G5" s="24">
         <v>0</v>
       </c>
-      <c r="H5" s="14">
+      <c r="H5" s="24">
         <v>0</v>
       </c>
-      <c r="I5" s="28">
+      <c r="I5" s="38">
         <v>0</v>
       </c>
     </row>
     <row r="6" ht="16.5" spans="1:9">
-      <c r="A6" s="20" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" s="21">
+      <c r="A6" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="31">
         <v>512</v>
       </c>
-      <c r="C6" s="14">
+      <c r="C6" s="24">
         <v>30</v>
       </c>
-      <c r="D6" s="14">
+      <c r="D6" s="24">
         <v>70</v>
       </c>
-      <c r="E6" s="14">
+      <c r="E6" s="24">
         <v>100</v>
       </c>
-      <c r="F6" s="14">
+      <c r="F6" s="24">
         <v>100</v>
       </c>
-      <c r="G6" s="14">
+      <c r="G6" s="24">
         <v>0</v>
       </c>
-      <c r="H6" s="14">
+      <c r="H6" s="24">
         <v>0</v>
       </c>
-      <c r="I6" s="28">
+      <c r="I6" s="38">
         <v>0</v>
       </c>
     </row>
     <row r="7" ht="16.5" spans="1:9">
-      <c r="A7" s="20" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" s="21">
+      <c r="A7" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="31">
         <v>1024</v>
       </c>
-      <c r="C7" s="14">
+      <c r="C7" s="24">
         <v>50</v>
       </c>
-      <c r="D7" s="14">
+      <c r="D7" s="24">
         <v>50</v>
       </c>
-      <c r="E7" s="14">
+      <c r="E7" s="24">
         <v>100</v>
       </c>
-      <c r="F7" s="14">
+      <c r="F7" s="24">
         <v>100</v>
       </c>
-      <c r="G7" s="14">
+      <c r="G7" s="24">
         <v>0</v>
       </c>
-      <c r="H7" s="14">
+      <c r="H7" s="24">
         <v>0</v>
       </c>
-      <c r="I7" s="28">
+      <c r="I7" s="38">
         <v>0</v>
       </c>
     </row>
     <row r="8" ht="16.5" spans="1:9">
-      <c r="A8" s="20" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8" s="21">
+      <c r="A8" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="31">
         <v>2048</v>
       </c>
-      <c r="C8" s="14">
+      <c r="C8" s="24">
         <v>70</v>
       </c>
-      <c r="D8" s="14">
+      <c r="D8" s="24">
         <v>80</v>
       </c>
-      <c r="E8" s="14">
+      <c r="E8" s="24">
         <v>100</v>
       </c>
-      <c r="F8" s="14">
+      <c r="F8" s="24">
         <v>40</v>
       </c>
-      <c r="G8" s="14">
-        <v>10</v>
-      </c>
-      <c r="H8" s="14">
+      <c r="G8" s="24">
+        <v>10</v>
+      </c>
+      <c r="H8" s="24">
         <v>0</v>
       </c>
-      <c r="I8" s="28">
+      <c r="I8" s="38">
         <v>0</v>
       </c>
     </row>
     <row r="9" ht="16.5" spans="1:9">
-      <c r="A9" s="20" t="s">
-        <v>6</v>
-      </c>
-      <c r="B9" s="22">
+      <c r="A9" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="32">
         <v>4096</v>
       </c>
-      <c r="C9" s="23">
+      <c r="C9" s="33">
         <v>50</v>
       </c>
-      <c r="D9" s="23">
+      <c r="D9" s="33">
         <v>80</v>
       </c>
-      <c r="E9" s="23">
+      <c r="E9" s="33">
         <v>100</v>
       </c>
-      <c r="F9" s="23">
+      <c r="F9" s="33">
         <v>50</v>
       </c>
-      <c r="G9" s="23">
-        <v>10</v>
-      </c>
-      <c r="H9" s="23">
-        <v>10</v>
-      </c>
-      <c r="I9" s="28">
+      <c r="G9" s="33">
+        <v>10</v>
+      </c>
+      <c r="H9" s="33">
+        <v>10</v>
+      </c>
+      <c r="I9" s="38">
         <v>0</v>
       </c>
     </row>
     <row r="10" ht="16.5" spans="1:9">
-      <c r="A10" s="24" t="s">
+      <c r="A10" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="25">
+      <c r="B10" s="35">
         <v>8192</v>
       </c>
-      <c r="C10" s="26">
+      <c r="C10" s="36">
         <v>60</v>
       </c>
-      <c r="D10" s="26">
+      <c r="D10" s="36">
         <v>60</v>
       </c>
-      <c r="E10" s="26">
+      <c r="E10" s="36">
         <v>100</v>
       </c>
-      <c r="F10" s="26">
+      <c r="F10" s="36">
         <v>50</v>
       </c>
-      <c r="G10" s="26">
-        <v>10</v>
-      </c>
-      <c r="H10" s="26">
-        <v>10</v>
-      </c>
-      <c r="I10" s="29">
+      <c r="G10" s="36">
+        <v>10</v>
+      </c>
+      <c r="H10" s="36">
+        <v>10</v>
+      </c>
+      <c r="I10" s="39">
         <v>10</v>
       </c>
     </row>
@@ -1906,81 +2013,81 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="26" customHeight="1" outlineLevelRow="6" outlineLevelCol="2"/>
   <cols>
-    <col min="1" max="16384" width="9" style="14"/>
+    <col min="1" max="16384" width="9" style="24"/>
   </cols>
   <sheetData>
     <row r="1" customHeight="1" spans="1:3">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16" t="s">
+      <c r="B1" s="26"/>
+      <c r="C1" s="26" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="2" customHeight="1" spans="1:3">
-      <c r="A2" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2" s="16">
+      <c r="A2" s="25" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="26">
         <v>1</v>
       </c>
-      <c r="C2" s="16">
+      <c r="C2" s="26">
         <v>200</v>
       </c>
     </row>
     <row r="3" customHeight="1" spans="1:3">
-      <c r="A3" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" s="16">
+      <c r="A3" s="25" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="26">
         <v>3</v>
       </c>
-      <c r="C3" s="16">
+      <c r="C3" s="26">
         <v>500</v>
       </c>
     </row>
     <row r="4" customHeight="1" spans="1:3">
-      <c r="A4" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" s="16">
-        <v>10</v>
-      </c>
-      <c r="C4" s="16">
+      <c r="A4" s="25" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="26">
+        <v>10</v>
+      </c>
+      <c r="C4" s="26">
         <v>1000</v>
       </c>
     </row>
     <row r="5" customHeight="1" spans="1:3">
-      <c r="A5" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" s="16">
+      <c r="A5" s="25" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="26">
         <v>20</v>
       </c>
-      <c r="C5" s="16">
+      <c r="C5" s="26">
         <v>2000</v>
       </c>
     </row>
     <row r="6" customHeight="1" spans="1:3">
-      <c r="A6" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" s="16">
+      <c r="A6" s="25" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="26">
         <v>50</v>
       </c>
-      <c r="C6" s="16">
+      <c r="C6" s="26">
         <v>3000</v>
       </c>
     </row>
     <row r="7" customHeight="1" spans="1:3">
-      <c r="A7" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" s="16">
+      <c r="A7" s="25" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="26">
         <v>999</v>
       </c>
-      <c r="C7" s="16">
+      <c r="C7" s="26">
         <v>5000</v>
       </c>
     </row>
@@ -2006,542 +2113,542 @@
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="7"/>
   <sheetData>
     <row r="1" ht="17.25" spans="1:8">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8" t="s">
+      <c r="B1" s="18"/>
+      <c r="C1" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="8"/>
-      <c r="E1" s="9" t="s">
+      <c r="D1" s="18"/>
+      <c r="E1" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="F1" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="G1" s="8"/>
-      <c r="H1" s="9" t="s">
+      <c r="G1" s="18"/>
+      <c r="H1" s="19" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="2" ht="18" spans="1:8">
-      <c r="A2" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" s="11">
+      <c r="A2" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="21">
         <v>1000</v>
       </c>
-      <c r="C2" s="8">
+      <c r="C2" s="18">
         <v>1000</v>
       </c>
-      <c r="D2" s="8">
+      <c r="D2" s="18">
         <v>1500</v>
       </c>
-      <c r="E2" s="8">
+      <c r="E2" s="18">
         <v>100</v>
       </c>
-      <c r="F2" s="8">
-        <v>150</v>
-      </c>
-      <c r="G2" s="8">
-        <v>250</v>
-      </c>
-      <c r="H2" s="8">
+      <c r="F2" s="18">
+        <v>150</v>
+      </c>
+      <c r="G2" s="18">
+        <v>250</v>
+      </c>
+      <c r="H2" s="18">
         <v>0</v>
       </c>
     </row>
     <row r="3" ht="18" spans="1:8">
-      <c r="A3" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="12">
+      <c r="A3" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="22">
         <v>2000</v>
       </c>
-      <c r="C3" s="13">
+      <c r="C3" s="23">
         <v>500</v>
       </c>
-      <c r="D3" s="13">
+      <c r="D3" s="23">
         <v>1000</v>
       </c>
-      <c r="E3" s="13">
+      <c r="E3" s="23">
         <v>100</v>
       </c>
-      <c r="F3" s="13">
-        <v>150</v>
-      </c>
-      <c r="G3" s="13">
-        <v>250</v>
-      </c>
-      <c r="H3" s="13">
+      <c r="F3" s="23">
+        <v>150</v>
+      </c>
+      <c r="G3" s="23">
+        <v>250</v>
+      </c>
+      <c r="H3" s="23">
         <v>0</v>
       </c>
     </row>
     <row r="4" ht="18" spans="1:8">
-      <c r="A4" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="12">
+      <c r="A4" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="22">
         <v>3000</v>
       </c>
-      <c r="C4" s="13">
+      <c r="C4" s="23">
         <v>300</v>
       </c>
-      <c r="D4" s="13">
+      <c r="D4" s="23">
         <v>500</v>
       </c>
-      <c r="E4" s="13">
+      <c r="E4" s="23">
         <v>100</v>
       </c>
-      <c r="F4" s="13">
-        <v>150</v>
-      </c>
-      <c r="G4" s="13">
-        <v>250</v>
-      </c>
-      <c r="H4" s="13">
+      <c r="F4" s="23">
+        <v>150</v>
+      </c>
+      <c r="G4" s="23">
+        <v>250</v>
+      </c>
+      <c r="H4" s="23">
         <v>0</v>
       </c>
     </row>
     <row r="5" ht="18" spans="1:8">
-      <c r="A5" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="12">
+      <c r="A5" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="22">
         <v>4000</v>
       </c>
-      <c r="C5" s="13">
+      <c r="C5" s="23">
         <v>200</v>
       </c>
-      <c r="D5" s="13">
+      <c r="D5" s="23">
         <v>400</v>
       </c>
-      <c r="E5" s="13">
+      <c r="E5" s="23">
         <v>80</v>
       </c>
-      <c r="F5" s="13">
-        <v>150</v>
-      </c>
-      <c r="G5" s="13">
-        <v>250</v>
-      </c>
-      <c r="H5" s="13">
+      <c r="F5" s="23">
+        <v>150</v>
+      </c>
+      <c r="G5" s="23">
+        <v>250</v>
+      </c>
+      <c r="H5" s="23">
         <v>0</v>
       </c>
     </row>
     <row r="6" ht="18" spans="1:8">
-      <c r="A6" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" s="12">
+      <c r="A6" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="22">
         <v>5000</v>
       </c>
-      <c r="C6" s="13">
+      <c r="C6" s="23">
         <v>100</v>
       </c>
-      <c r="D6" s="13">
+      <c r="D6" s="23">
         <v>120</v>
       </c>
-      <c r="E6" s="13">
+      <c r="E6" s="23">
         <v>80</v>
       </c>
-      <c r="F6" s="13">
-        <v>150</v>
-      </c>
-      <c r="G6" s="13">
-        <v>250</v>
-      </c>
-      <c r="H6" s="13">
+      <c r="F6" s="23">
+        <v>150</v>
+      </c>
+      <c r="G6" s="23">
+        <v>250</v>
+      </c>
+      <c r="H6" s="23">
         <v>15</v>
       </c>
     </row>
     <row r="7" ht="18" spans="1:8">
-      <c r="A7" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" s="12">
+      <c r="A7" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="22">
         <v>5500</v>
       </c>
-      <c r="C7" s="13">
+      <c r="C7" s="23">
         <v>50</v>
       </c>
-      <c r="D7" s="13">
+      <c r="D7" s="23">
         <v>70</v>
       </c>
-      <c r="E7" s="13">
+      <c r="E7" s="23">
         <v>80</v>
       </c>
-      <c r="F7" s="13">
-        <v>150</v>
-      </c>
-      <c r="G7" s="13">
-        <v>250</v>
-      </c>
-      <c r="H7" s="13">
+      <c r="F7" s="23">
+        <v>150</v>
+      </c>
+      <c r="G7" s="23">
+        <v>250</v>
+      </c>
+      <c r="H7" s="23">
         <v>15</v>
       </c>
     </row>
     <row r="8" ht="18" spans="1:8">
-      <c r="A8" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8" s="12">
+      <c r="A8" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="22">
         <v>6000</v>
       </c>
-      <c r="C8" s="13">
+      <c r="C8" s="23">
         <v>20</v>
       </c>
-      <c r="D8" s="13">
+      <c r="D8" s="23">
         <v>50</v>
       </c>
-      <c r="E8" s="13">
+      <c r="E8" s="23">
         <v>80</v>
       </c>
-      <c r="F8" s="13">
-        <v>150</v>
-      </c>
-      <c r="G8" s="13">
-        <v>250</v>
-      </c>
-      <c r="H8" s="13">
+      <c r="F8" s="23">
+        <v>150</v>
+      </c>
+      <c r="G8" s="23">
+        <v>250</v>
+      </c>
+      <c r="H8" s="23">
         <v>15</v>
       </c>
     </row>
     <row r="9" ht="18" spans="1:8">
-      <c r="A9" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="B9" s="12">
+      <c r="A9" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="22">
         <v>6500</v>
       </c>
-      <c r="C9" s="13">
-        <v>10</v>
-      </c>
-      <c r="D9" s="13">
+      <c r="C9" s="23">
+        <v>10</v>
+      </c>
+      <c r="D9" s="23">
         <v>20</v>
       </c>
-      <c r="E9" s="13">
+      <c r="E9" s="23">
         <v>50</v>
       </c>
-      <c r="F9" s="13">
-        <v>150</v>
-      </c>
-      <c r="G9" s="13">
-        <v>250</v>
-      </c>
-      <c r="H9" s="13">
+      <c r="F9" s="23">
+        <v>150</v>
+      </c>
+      <c r="G9" s="23">
+        <v>250</v>
+      </c>
+      <c r="H9" s="23">
         <v>40</v>
       </c>
     </row>
     <row r="10" ht="18" spans="1:8">
-      <c r="A10" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="B10" s="12">
+      <c r="A10" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" s="22">
         <v>7000</v>
       </c>
-      <c r="C10" s="13">
-        <v>10</v>
-      </c>
-      <c r="D10" s="13">
-        <v>10</v>
-      </c>
-      <c r="E10" s="13">
+      <c r="C10" s="23">
+        <v>10</v>
+      </c>
+      <c r="D10" s="23">
+        <v>10</v>
+      </c>
+      <c r="E10" s="23">
         <v>50</v>
       </c>
-      <c r="F10" s="13">
-        <v>150</v>
-      </c>
-      <c r="G10" s="13">
-        <v>250</v>
-      </c>
-      <c r="H10" s="13">
+      <c r="F10" s="23">
+        <v>150</v>
+      </c>
+      <c r="G10" s="23">
+        <v>250</v>
+      </c>
+      <c r="H10" s="23">
         <v>40</v>
       </c>
     </row>
     <row r="11" ht="18" spans="1:8">
-      <c r="A11" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="B11" s="12">
+      <c r="A11" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11" s="22">
         <v>7500</v>
       </c>
-      <c r="C11" s="13">
-        <v>10</v>
-      </c>
-      <c r="D11" s="13">
-        <v>10</v>
-      </c>
-      <c r="E11" s="13">
+      <c r="C11" s="23">
+        <v>10</v>
+      </c>
+      <c r="D11" s="23">
+        <v>10</v>
+      </c>
+      <c r="E11" s="23">
         <v>50</v>
       </c>
-      <c r="F11" s="13">
-        <v>150</v>
-      </c>
-      <c r="G11" s="13">
-        <v>250</v>
-      </c>
-      <c r="H11" s="13">
+      <c r="F11" s="23">
+        <v>150</v>
+      </c>
+      <c r="G11" s="23">
+        <v>250</v>
+      </c>
+      <c r="H11" s="23">
         <v>40</v>
       </c>
     </row>
     <row r="12" ht="18" spans="1:8">
-      <c r="A12" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="B12" s="12">
+      <c r="A12" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="B12" s="22">
         <v>8000</v>
       </c>
-      <c r="C12" s="13">
-        <v>10</v>
-      </c>
-      <c r="D12" s="13">
-        <v>10</v>
-      </c>
-      <c r="E12" s="13">
+      <c r="C12" s="23">
+        <v>10</v>
+      </c>
+      <c r="D12" s="23">
+        <v>10</v>
+      </c>
+      <c r="E12" s="23">
         <v>30</v>
       </c>
-      <c r="F12" s="13">
-        <v>150</v>
-      </c>
-      <c r="G12" s="13">
-        <v>250</v>
-      </c>
-      <c r="H12" s="13">
+      <c r="F12" s="23">
+        <v>150</v>
+      </c>
+      <c r="G12" s="23">
+        <v>250</v>
+      </c>
+      <c r="H12" s="23">
         <v>50</v>
       </c>
     </row>
     <row r="13" ht="18" spans="1:8">
-      <c r="A13" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="B13" s="12">
+      <c r="A13" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="B13" s="22">
         <v>8200</v>
       </c>
-      <c r="C13" s="13">
-        <v>10</v>
-      </c>
-      <c r="D13" s="13">
-        <v>10</v>
-      </c>
-      <c r="E13" s="13">
+      <c r="C13" s="23">
+        <v>10</v>
+      </c>
+      <c r="D13" s="23">
+        <v>10</v>
+      </c>
+      <c r="E13" s="23">
         <v>30</v>
       </c>
-      <c r="F13" s="13">
-        <v>150</v>
-      </c>
-      <c r="G13" s="13">
-        <v>250</v>
-      </c>
-      <c r="H13" s="13">
+      <c r="F13" s="23">
+        <v>150</v>
+      </c>
+      <c r="G13" s="23">
+        <v>250</v>
+      </c>
+      <c r="H13" s="23">
         <v>50</v>
       </c>
     </row>
     <row r="14" ht="18" spans="1:8">
-      <c r="A14" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="B14" s="12">
+      <c r="A14" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="B14" s="22">
         <v>8400</v>
       </c>
-      <c r="C14" s="13">
-        <v>10</v>
-      </c>
-      <c r="D14" s="13">
-        <v>10</v>
-      </c>
-      <c r="E14" s="13">
+      <c r="C14" s="23">
+        <v>10</v>
+      </c>
+      <c r="D14" s="23">
+        <v>10</v>
+      </c>
+      <c r="E14" s="23">
         <v>30</v>
       </c>
-      <c r="F14" s="13">
-        <v>150</v>
-      </c>
-      <c r="G14" s="13">
-        <v>250</v>
-      </c>
-      <c r="H14" s="13">
+      <c r="F14" s="23">
+        <v>150</v>
+      </c>
+      <c r="G14" s="23">
+        <v>250</v>
+      </c>
+      <c r="H14" s="23">
         <v>50</v>
       </c>
     </row>
     <row r="15" ht="18" spans="1:8">
-      <c r="A15" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="B15" s="12">
+      <c r="A15" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="B15" s="22">
         <v>8600</v>
       </c>
-      <c r="C15" s="13">
-        <v>10</v>
-      </c>
-      <c r="D15" s="13">
-        <v>10</v>
-      </c>
-      <c r="E15" s="13">
-        <v>10</v>
-      </c>
-      <c r="F15" s="13">
-        <v>150</v>
-      </c>
-      <c r="G15" s="13">
-        <v>250</v>
-      </c>
-      <c r="H15" s="13">
+      <c r="C15" s="23">
+        <v>10</v>
+      </c>
+      <c r="D15" s="23">
+        <v>10</v>
+      </c>
+      <c r="E15" s="23">
+        <v>10</v>
+      </c>
+      <c r="F15" s="23">
+        <v>150</v>
+      </c>
+      <c r="G15" s="23">
+        <v>250</v>
+      </c>
+      <c r="H15" s="23">
         <v>70</v>
       </c>
     </row>
     <row r="16" ht="18" spans="1:8">
-      <c r="A16" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="B16" s="12">
+      <c r="A16" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="B16" s="22">
         <v>8800</v>
       </c>
-      <c r="C16" s="13">
-        <v>10</v>
-      </c>
-      <c r="D16" s="13">
-        <v>10</v>
-      </c>
-      <c r="E16" s="13">
-        <v>10</v>
-      </c>
-      <c r="F16" s="13">
-        <v>150</v>
-      </c>
-      <c r="G16" s="13">
-        <v>250</v>
-      </c>
-      <c r="H16" s="13">
+      <c r="C16" s="23">
+        <v>10</v>
+      </c>
+      <c r="D16" s="23">
+        <v>10</v>
+      </c>
+      <c r="E16" s="23">
+        <v>10</v>
+      </c>
+      <c r="F16" s="23">
+        <v>150</v>
+      </c>
+      <c r="G16" s="23">
+        <v>250</v>
+      </c>
+      <c r="H16" s="23">
         <v>70</v>
       </c>
     </row>
     <row r="17" ht="18" spans="1:8">
-      <c r="A17" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="B17" s="12">
+      <c r="A17" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="B17" s="22">
         <v>9000</v>
       </c>
-      <c r="C17" s="13">
-        <v>10</v>
-      </c>
-      <c r="D17" s="13">
-        <v>10</v>
-      </c>
-      <c r="E17" s="13">
-        <v>10</v>
-      </c>
-      <c r="F17" s="13">
-        <v>150</v>
-      </c>
-      <c r="G17" s="13">
-        <v>250</v>
-      </c>
-      <c r="H17" s="13">
+      <c r="C17" s="23">
+        <v>10</v>
+      </c>
+      <c r="D17" s="23">
+        <v>10</v>
+      </c>
+      <c r="E17" s="23">
+        <v>10</v>
+      </c>
+      <c r="F17" s="23">
+        <v>150</v>
+      </c>
+      <c r="G17" s="23">
+        <v>250</v>
+      </c>
+      <c r="H17" s="23">
         <v>70</v>
       </c>
     </row>
     <row r="18" ht="18" spans="1:8">
-      <c r="A18" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="B18" s="12">
+      <c r="A18" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="B18" s="22">
         <v>9200</v>
       </c>
-      <c r="C18" s="13">
-        <v>10</v>
-      </c>
-      <c r="D18" s="13">
-        <v>10</v>
-      </c>
-      <c r="E18" s="13">
+      <c r="C18" s="23">
+        <v>10</v>
+      </c>
+      <c r="D18" s="23">
+        <v>10</v>
+      </c>
+      <c r="E18" s="23">
         <v>0</v>
       </c>
-      <c r="F18" s="13">
-        <v>150</v>
-      </c>
-      <c r="G18" s="13">
-        <v>250</v>
-      </c>
-      <c r="H18" s="13">
+      <c r="F18" s="23">
+        <v>150</v>
+      </c>
+      <c r="G18" s="23">
+        <v>250</v>
+      </c>
+      <c r="H18" s="23">
         <v>70</v>
       </c>
     </row>
     <row r="19" ht="18" spans="1:8">
-      <c r="A19" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="B19" s="12">
+      <c r="A19" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="B19" s="22">
         <v>9400</v>
       </c>
-      <c r="C19" s="13">
-        <v>10</v>
-      </c>
-      <c r="D19" s="13">
-        <v>10</v>
-      </c>
-      <c r="E19" s="13">
+      <c r="C19" s="23">
+        <v>10</v>
+      </c>
+      <c r="D19" s="23">
+        <v>10</v>
+      </c>
+      <c r="E19" s="23">
         <v>0</v>
       </c>
-      <c r="F19" s="13">
-        <v>150</v>
-      </c>
-      <c r="G19" s="13">
-        <v>250</v>
-      </c>
-      <c r="H19" s="13">
+      <c r="F19" s="23">
+        <v>150</v>
+      </c>
+      <c r="G19" s="23">
+        <v>250</v>
+      </c>
+      <c r="H19" s="23">
         <v>70</v>
       </c>
     </row>
     <row r="20" ht="18" spans="1:8">
-      <c r="A20" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="B20" s="12">
+      <c r="A20" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="B20" s="22">
         <v>9600</v>
       </c>
-      <c r="C20" s="13">
-        <v>10</v>
-      </c>
-      <c r="D20" s="13">
-        <v>10</v>
-      </c>
-      <c r="E20" s="13">
+      <c r="C20" s="23">
+        <v>10</v>
+      </c>
+      <c r="D20" s="23">
+        <v>10</v>
+      </c>
+      <c r="E20" s="23">
         <v>0</v>
       </c>
-      <c r="F20" s="13">
-        <v>150</v>
-      </c>
-      <c r="G20" s="13">
-        <v>250</v>
-      </c>
-      <c r="H20" s="13">
+      <c r="F20" s="23">
+        <v>150</v>
+      </c>
+      <c r="G20" s="23">
+        <v>250</v>
+      </c>
+      <c r="H20" s="23">
         <v>70</v>
       </c>
     </row>
     <row r="21" ht="18" spans="1:8">
-      <c r="A21" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="B21" s="12">
+      <c r="A21" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="B21" s="22">
         <v>10000</v>
       </c>
-      <c r="C21" s="13">
-        <v>10</v>
-      </c>
-      <c r="D21" s="13">
-        <v>10</v>
-      </c>
-      <c r="E21" s="13">
+      <c r="C21" s="23">
+        <v>10</v>
+      </c>
+      <c r="D21" s="23">
+        <v>10</v>
+      </c>
+      <c r="E21" s="23">
         <v>0</v>
       </c>
-      <c r="F21" s="13">
-        <v>150</v>
-      </c>
-      <c r="G21" s="13">
-        <v>250</v>
-      </c>
-      <c r="H21" s="13">
+      <c r="F21" s="23">
+        <v>150</v>
+      </c>
+      <c r="G21" s="23">
+        <v>250</v>
+      </c>
+      <c r="H21" s="23">
         <v>70</v>
       </c>
     </row>
@@ -2573,223 +2680,223 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="16" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="B2" s="6">
+      <c r="B2" s="16">
         <v>1000</v>
       </c>
-      <c r="C2" s="6">
-        <v>10</v>
-      </c>
-      <c r="D2" s="6">
+      <c r="C2" s="16">
+        <v>10</v>
+      </c>
+      <c r="D2" s="16">
         <v>-1</v>
       </c>
-      <c r="E2" s="6">
+      <c r="E2" s="16">
         <v>-1</v>
       </c>
     </row>
     <row r="3" spans="1:5">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="B3" s="6">
+      <c r="B3" s="16">
         <v>2</v>
       </c>
-      <c r="C3" s="6">
+      <c r="C3" s="16">
         <v>100</v>
       </c>
-      <c r="D3" s="6">
+      <c r="D3" s="16">
         <v>-1</v>
       </c>
-      <c r="E3" s="6">
+      <c r="E3" s="16">
         <v>-1</v>
       </c>
     </row>
     <row r="4" spans="1:5">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="B4" s="6">
+      <c r="B4" s="16">
         <v>50</v>
       </c>
-      <c r="C4" s="6">
+      <c r="C4" s="16">
         <v>200</v>
       </c>
-      <c r="D4" s="6">
+      <c r="D4" s="16">
         <v>-1</v>
       </c>
-      <c r="E4" s="6">
+      <c r="E4" s="16">
         <v>-1</v>
       </c>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="B5" s="6">
+      <c r="B5" s="16">
         <v>2</v>
       </c>
-      <c r="C5" s="6">
+      <c r="C5" s="16">
         <v>40</v>
       </c>
-      <c r="D5" s="6">
+      <c r="D5" s="16">
         <v>-1</v>
       </c>
-      <c r="E5" s="6">
+      <c r="E5" s="16">
         <v>-1</v>
       </c>
     </row>
     <row r="6" spans="1:5">
-      <c r="A6" s="6" t="s">
+      <c r="A6" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="6">
+      <c r="B6" s="16">
         <v>100</v>
       </c>
-      <c r="C6" s="6">
+      <c r="C6" s="16">
         <v>100</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="D6" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="E6" s="6">
+      <c r="E6" s="16">
         <v>3000</v>
       </c>
     </row>
     <row r="7" spans="1:5">
-      <c r="A7" s="6" t="s">
+      <c r="A7" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="B7" s="6">
+      <c r="B7" s="16">
         <v>2</v>
       </c>
-      <c r="C7" s="6">
+      <c r="C7" s="16">
         <v>40</v>
       </c>
-      <c r="D7" s="6">
+      <c r="D7" s="16">
         <v>-1</v>
       </c>
-      <c r="E7" s="6">
+      <c r="E7" s="16">
         <v>-1</v>
       </c>
     </row>
     <row r="8" spans="1:5">
-      <c r="A8" s="6" t="s">
+      <c r="A8" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="B8" s="6">
+      <c r="B8" s="16">
         <v>100</v>
       </c>
-      <c r="C8" s="6">
+      <c r="C8" s="16">
         <v>200</v>
       </c>
-      <c r="D8" s="6">
+      <c r="D8" s="16">
         <v>-1</v>
       </c>
-      <c r="E8" s="6">
+      <c r="E8" s="16">
         <v>-1</v>
       </c>
     </row>
     <row r="9" spans="1:5">
-      <c r="A9" s="6" t="s">
+      <c r="A9" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="B9" s="6">
+      <c r="B9" s="16">
         <v>100000</v>
       </c>
-      <c r="C9" s="6">
+      <c r="C9" s="16">
         <v>0</v>
       </c>
-      <c r="D9" s="6">
+      <c r="D9" s="16">
         <v>-1</v>
       </c>
-      <c r="E9" s="6">
+      <c r="E9" s="16">
         <v>-1</v>
       </c>
     </row>
     <row r="10" spans="1:5">
-      <c r="A10" s="6" t="s">
+      <c r="A10" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="B10" s="6">
+      <c r="B10" s="16">
         <v>1</v>
       </c>
-      <c r="C10" s="6">
+      <c r="C10" s="16">
         <v>40</v>
       </c>
-      <c r="D10" s="6">
+      <c r="D10" s="16">
         <v>-1</v>
       </c>
-      <c r="E10" s="6">
+      <c r="E10" s="16">
         <v>-1</v>
       </c>
     </row>
     <row r="11" spans="1:5">
-      <c r="A11" s="6" t="s">
+      <c r="A11" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="B11" s="6">
-        <v>10</v>
-      </c>
-      <c r="C11" s="6">
+      <c r="B11" s="16">
+        <v>10</v>
+      </c>
+      <c r="C11" s="16">
         <v>100</v>
       </c>
-      <c r="D11" s="6">
+      <c r="D11" s="16">
         <v>-1</v>
       </c>
-      <c r="E11" s="6">
+      <c r="E11" s="16">
         <v>9600</v>
       </c>
     </row>
     <row r="12" spans="1:5">
-      <c r="A12" s="6" t="s">
+      <c r="A12" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="B12" s="6">
+      <c r="B12" s="16">
         <v>200</v>
       </c>
-      <c r="C12" s="6">
+      <c r="C12" s="16">
         <v>40</v>
       </c>
-      <c r="D12" s="6">
+      <c r="D12" s="16">
         <v>-1</v>
       </c>
-      <c r="E12" s="6">
+      <c r="E12" s="16">
         <v>-1</v>
       </c>
     </row>
     <row r="13" spans="1:5">
-      <c r="A13" s="6" t="s">
+      <c r="A13" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="B13" s="6">
+      <c r="B13" s="16">
         <v>1</v>
       </c>
-      <c r="C13" s="6">
+      <c r="C13" s="16">
         <v>40</v>
       </c>
-      <c r="D13" s="6">
+      <c r="D13" s="16">
         <v>-1</v>
       </c>
-      <c r="E13" s="6">
+      <c r="E13" s="16">
         <v>-1</v>
       </c>
     </row>
@@ -2802,62 +2909,86 @@
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="3" outlineLevelCol="2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="3" outlineLevelCol="4"/>
   <cols>
-    <col min="3" max="3" width="16.75" customWidth="1"/>
+    <col min="4" max="4" width="16.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="17.25" spans="1:3">
-      <c r="A1" s="5" t="s">
+    <row r="1" ht="17.25" spans="1:5">
+      <c r="A1" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="13"/>
+      <c r="D1" s="12" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="2" ht="17.25" spans="1:3">
-      <c r="A2" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="B2" s="5">
+      <c r="E1" s="14"/>
+    </row>
+    <row r="2" ht="17.25" spans="1:5">
+      <c r="A2" s="15">
         <v>3</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="B2" s="15">
+        <v>3</v>
+      </c>
+      <c r="C2" s="15">
+        <v>3</v>
+      </c>
+      <c r="D2" s="15">
+        <v>200</v>
+      </c>
+      <c r="E2" s="15">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="3" ht="17.25" spans="1:5">
+      <c r="A3" s="15">
+        <v>10</v>
+      </c>
+      <c r="B3" s="15">
+        <v>3</v>
+      </c>
+      <c r="C3" s="15">
+        <v>10</v>
+      </c>
+      <c r="D3" s="15">
+        <v>150</v>
+      </c>
+      <c r="E3" s="15">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="4" ht="17.25" spans="1:5">
+      <c r="A4" s="15">
+        <v>9999</v>
+      </c>
+      <c r="B4" s="15">
         <v>30</v>
       </c>
-    </row>
-    <row r="3" ht="17.25" spans="1:3">
-      <c r="A3" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="4" ht="17.25" spans="1:3">
-      <c r="A4" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="B4" s="5">
+      <c r="C4" s="15">
         <v>30</v>
       </c>
-      <c r="C4" s="5" t="s">
-        <v>34</v>
+      <c r="D4" s="15">
+        <v>50</v>
+      </c>
+      <c r="E4" s="15">
+        <v>100</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="D1:E1"/>
+  </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
 </worksheet>
@@ -2866,88 +2997,98 @@
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:I23"/>
+  <dimension ref="A1:J23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="N31" sqref="N31:O31"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
   <cols>
-    <col min="3" max="4" width="9.25"/>
-    <col min="9" max="9" width="14.875" customWidth="1"/>
+    <col min="1" max="1" width="3.375" customWidth="1"/>
+    <col min="2" max="2" width="9.13333333333333" customWidth="1"/>
+    <col min="3" max="3" width="9.25"/>
+    <col min="4" max="4" width="9.25" customWidth="1"/>
+    <col min="5" max="5" width="4.75" customWidth="1"/>
+    <col min="6" max="6" width="4.375" customWidth="1"/>
+    <col min="7" max="8" width="5.875" customWidth="1"/>
+    <col min="9" max="9" width="8.35" customWidth="1"/>
+    <col min="10" max="10" width="8.44166666666667" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="18" customHeight="1" spans="1:9">
+    <row r="1" ht="18" customHeight="1" spans="1:10">
       <c r="A1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="7"/>
+    </row>
+    <row r="2" ht="18" customHeight="1" spans="1:10">
+      <c r="A2" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F2" s="3"/>
+      <c r="G2" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="7"/>
+    </row>
+    <row r="3" ht="17.25" spans="1:10">
+      <c r="A3" s="3"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="F3" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-    </row>
-    <row r="2" ht="18" customHeight="1" spans="1:9">
-      <c r="A2" s="1" t="s">
+      <c r="G3" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1" t="s">
+      <c r="H3" s="3"/>
+      <c r="I3" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-    </row>
-    <row r="3" ht="17.25" spans="1:9">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="4" ht="17.25" spans="1:9">
-      <c r="A4" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="3">
-        <v>10</v>
-      </c>
-      <c r="C4" s="3">
-        <v>10</v>
-      </c>
-      <c r="D4" s="3">
-        <v>10</v>
-      </c>
-      <c r="E4" s="1">
+      <c r="J3" s="9"/>
+    </row>
+    <row r="4" ht="17.25" spans="1:10">
+      <c r="A4" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="4">
+        <v>1000</v>
+      </c>
+      <c r="C4" s="4">
+        <v>10</v>
+      </c>
+      <c r="D4" s="4">
+        <v>10</v>
+      </c>
+      <c r="E4" s="3">
         <v>100</v>
       </c>
-      <c r="F4" s="1">
+      <c r="F4" s="3">
         <v>0</v>
       </c>
       <c r="G4" s="3">
@@ -2956,56 +3097,62 @@
       <c r="H4" s="3">
         <v>1500</v>
       </c>
-      <c r="I4" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="5" ht="17.25" spans="1:9">
-      <c r="A5" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="3">
+      <c r="I4" s="10">
+        <v>150</v>
+      </c>
+      <c r="J4" s="10">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="5" ht="17.25" spans="1:10">
+      <c r="A5" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="4">
+        <v>2000</v>
+      </c>
+      <c r="C5" s="5">
         <v>20</v>
       </c>
-      <c r="C5" s="4">
+      <c r="D5" s="5">
         <v>20</v>
       </c>
-      <c r="D5" s="4">
+      <c r="E5" s="3">
+        <v>100</v>
+      </c>
+      <c r="F5" s="3">
+        <v>0</v>
+      </c>
+      <c r="G5" s="6">
+        <v>500</v>
+      </c>
+      <c r="H5" s="6">
+        <v>1000</v>
+      </c>
+      <c r="I5" s="3">
+        <v>150</v>
+      </c>
+      <c r="J5" s="3">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="6" ht="17.25" spans="1:10">
+      <c r="A6" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="4">
+        <v>3000</v>
+      </c>
+      <c r="C6" s="5">
         <v>20</v>
       </c>
-      <c r="E5" s="1">
+      <c r="D6" s="5">
+        <v>20</v>
+      </c>
+      <c r="E6" s="3">
         <v>100</v>
       </c>
-      <c r="F5" s="1">
-        <v>0</v>
-      </c>
-      <c r="G5" s="4">
-        <v>500</v>
-      </c>
-      <c r="H5" s="4">
-        <v>1000</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="6" ht="17.25" spans="1:9">
-      <c r="A6" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" s="3">
-        <v>30</v>
-      </c>
-      <c r="C6" s="4">
-        <v>20</v>
-      </c>
-      <c r="D6" s="4">
-        <v>20</v>
-      </c>
-      <c r="E6" s="1">
-        <v>100</v>
-      </c>
-      <c r="F6" s="1">
+      <c r="F6" s="3">
         <v>0</v>
       </c>
       <c r="G6" s="3">
@@ -3014,27 +3161,30 @@
       <c r="H6" s="3">
         <v>150</v>
       </c>
-      <c r="I6" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="7" ht="17.25" spans="1:9">
-      <c r="A7" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" s="3">
-        <v>40</v>
-      </c>
-      <c r="C7" s="4">
+      <c r="I6" s="3">
+        <v>150</v>
+      </c>
+      <c r="J6" s="3">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="7" ht="17.25" spans="1:10">
+      <c r="A7" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="4">
+        <v>4000</v>
+      </c>
+      <c r="C7" s="5">
         <v>20</v>
       </c>
-      <c r="D7" s="4">
+      <c r="D7" s="5">
         <v>20</v>
       </c>
-      <c r="E7" s="1">
+      <c r="E7" s="3">
         <v>80</v>
       </c>
-      <c r="F7" s="2">
+      <c r="F7" s="6">
         <v>0</v>
       </c>
       <c r="G7" s="3">
@@ -3043,27 +3193,30 @@
       <c r="H7" s="3">
         <v>120</v>
       </c>
-      <c r="I7" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="8" ht="17.25" spans="1:9">
-      <c r="A8" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8" s="3">
-        <v>50</v>
-      </c>
-      <c r="C8" s="4">
+      <c r="I7" s="3">
+        <v>150</v>
+      </c>
+      <c r="J7" s="3">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="8" ht="17.25" spans="1:10">
+      <c r="A8" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="4">
+        <v>5000</v>
+      </c>
+      <c r="C8" s="5">
         <v>30</v>
       </c>
-      <c r="D8" s="4">
+      <c r="D8" s="5">
         <v>30</v>
       </c>
-      <c r="E8" s="1">
+      <c r="E8" s="3">
         <v>80</v>
       </c>
-      <c r="F8" s="1">
+      <c r="F8" s="3">
         <v>15</v>
       </c>
       <c r="G8" s="3">
@@ -3072,27 +3225,30 @@
       <c r="H8" s="3">
         <v>120</v>
       </c>
-      <c r="I8" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="9" ht="17.25" spans="1:9">
-      <c r="A9" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B9" s="3">
-        <v>55</v>
-      </c>
-      <c r="C9" s="4">
+      <c r="I8" s="3">
+        <v>150</v>
+      </c>
+      <c r="J8" s="3">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="9" ht="17.25" spans="1:10">
+      <c r="A9" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="4">
+        <v>5500</v>
+      </c>
+      <c r="C9" s="5">
         <v>30</v>
       </c>
-      <c r="D9" s="4">
+      <c r="D9" s="5">
         <v>30</v>
       </c>
-      <c r="E9" s="1">
+      <c r="E9" s="3">
         <v>80</v>
       </c>
-      <c r="F9" s="1">
+      <c r="F9" s="3">
         <v>15</v>
       </c>
       <c r="G9" s="3">
@@ -3101,27 +3257,30 @@
       <c r="H9" s="3">
         <v>70</v>
       </c>
-      <c r="I9" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="10" ht="17.25" spans="1:9">
-      <c r="A10" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B10" s="3">
-        <v>60</v>
-      </c>
-      <c r="C10" s="4">
+      <c r="I9" s="3">
+        <v>150</v>
+      </c>
+      <c r="J9" s="3">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="10" ht="17.25" spans="1:10">
+      <c r="A10" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" s="4">
+        <v>6000</v>
+      </c>
+      <c r="C10" s="5">
         <v>30</v>
       </c>
-      <c r="D10" s="4">
+      <c r="D10" s="5">
         <v>30</v>
       </c>
-      <c r="E10" s="1">
+      <c r="E10" s="3">
         <v>80</v>
       </c>
-      <c r="F10" s="1">
+      <c r="F10" s="3">
         <v>15</v>
       </c>
       <c r="G10" s="3">
@@ -3130,27 +3289,30 @@
       <c r="H10" s="3">
         <v>50</v>
       </c>
-      <c r="I10" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="11" ht="17.25" spans="1:9">
-      <c r="A11" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B11" s="3">
-        <v>65</v>
-      </c>
-      <c r="C11" s="4">
+      <c r="I10" s="3">
+        <v>150</v>
+      </c>
+      <c r="J10" s="3">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="11" ht="17.25" spans="1:10">
+      <c r="A11" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11" s="4">
+        <v>6500</v>
+      </c>
+      <c r="C11" s="5">
         <v>30</v>
       </c>
-      <c r="D11" s="4">
+      <c r="D11" s="5">
         <v>30</v>
       </c>
-      <c r="E11" s="1">
+      <c r="E11" s="3">
         <v>50</v>
       </c>
-      <c r="F11" s="1">
+      <c r="F11" s="3">
         <v>40</v>
       </c>
       <c r="G11" s="3">
@@ -3159,27 +3321,30 @@
       <c r="H11" s="3">
         <v>20</v>
       </c>
-      <c r="I11" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="12" ht="17.25" spans="1:9">
-      <c r="A12" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B12" s="3">
-        <v>70</v>
-      </c>
-      <c r="C12" s="4">
+      <c r="I11" s="3">
+        <v>150</v>
+      </c>
+      <c r="J11" s="3">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="12" ht="17.25" spans="1:10">
+      <c r="A12" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B12" s="4">
+        <v>7000</v>
+      </c>
+      <c r="C12" s="5">
         <v>50</v>
       </c>
-      <c r="D12" s="4">
+      <c r="D12" s="5">
         <v>50</v>
       </c>
-      <c r="E12" s="1">
+      <c r="E12" s="3">
         <v>50</v>
       </c>
-      <c r="F12" s="1">
+      <c r="F12" s="3">
         <v>40</v>
       </c>
       <c r="G12" s="3">
@@ -3188,85 +3353,94 @@
       <c r="H12" s="3">
         <v>15</v>
       </c>
-      <c r="I12" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="13" ht="17.25" spans="1:9">
-      <c r="A13" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B13" s="3">
-        <v>75</v>
-      </c>
-      <c r="C13" s="4">
+      <c r="I12" s="3">
+        <v>150</v>
+      </c>
+      <c r="J12" s="3">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="13" ht="17.25" spans="1:10">
+      <c r="A13" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B13" s="4">
+        <v>7500</v>
+      </c>
+      <c r="C13" s="5">
         <v>50</v>
       </c>
-      <c r="D13" s="4">
+      <c r="D13" s="5">
         <v>50</v>
       </c>
-      <c r="E13" s="1">
+      <c r="E13" s="3">
         <v>50</v>
       </c>
-      <c r="F13" s="1">
+      <c r="F13" s="3">
         <v>40</v>
       </c>
       <c r="G13" s="3">
         <v>5</v>
       </c>
-      <c r="H13" s="4">
+      <c r="H13" s="6">
         <v>8</v>
       </c>
-      <c r="I13" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="14" ht="17.25" spans="1:9">
-      <c r="A14" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B14" s="3">
-        <v>80</v>
-      </c>
-      <c r="C14" s="4">
+      <c r="I13" s="3">
+        <v>150</v>
+      </c>
+      <c r="J13" s="3">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="14" ht="17.25" spans="1:10">
+      <c r="A14" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B14" s="4">
+        <v>8000</v>
+      </c>
+      <c r="C14" s="5">
         <v>100</v>
       </c>
-      <c r="D14" s="4">
+      <c r="D14" s="5">
         <v>100</v>
       </c>
-      <c r="E14" s="1">
+      <c r="E14" s="3">
         <v>30</v>
       </c>
-      <c r="F14" s="1">
+      <c r="F14" s="3">
         <v>50</v>
       </c>
-      <c r="G14" s="4">
+      <c r="G14" s="6">
         <v>3</v>
       </c>
-      <c r="H14" s="4">
+      <c r="H14" s="6">
         <v>5</v>
       </c>
-      <c r="I14" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="15" ht="17.25" spans="1:9">
-      <c r="A15" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B15" s="3">
-        <v>82</v>
-      </c>
-      <c r="C15" s="4">
+      <c r="I14" s="3">
+        <v>150</v>
+      </c>
+      <c r="J14" s="3">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="15" ht="17.25" spans="1:10">
+      <c r="A15" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B15" s="4">
+        <v>8200</v>
+      </c>
+      <c r="C15" s="5">
         <v>200</v>
       </c>
-      <c r="D15" s="4">
+      <c r="D15" s="5">
         <v>200</v>
       </c>
-      <c r="E15" s="1">
+      <c r="E15" s="3">
         <v>30</v>
       </c>
-      <c r="F15" s="1">
+      <c r="F15" s="3">
         <v>50</v>
       </c>
       <c r="G15" s="3">
@@ -3275,27 +3449,30 @@
       <c r="H15" s="3">
         <v>3</v>
       </c>
-      <c r="I15" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="16" ht="17.25" spans="1:9">
+      <c r="I15" s="3">
+        <v>150</v>
+      </c>
+      <c r="J15" s="3">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="16" ht="17.25" spans="1:10">
       <c r="A16" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B16" s="3">
-        <v>84</v>
-      </c>
-      <c r="C16" s="4">
+      <c r="B16" s="4">
+        <v>8400</v>
+      </c>
+      <c r="C16" s="5">
         <v>200</v>
       </c>
-      <c r="D16" s="4">
+      <c r="D16" s="5">
         <v>200</v>
       </c>
-      <c r="E16" s="1">
+      <c r="E16" s="3">
         <v>30</v>
       </c>
-      <c r="F16" s="1">
+      <c r="F16" s="3">
         <v>50</v>
       </c>
       <c r="G16" s="3">
@@ -3304,27 +3481,30 @@
       <c r="H16" s="3">
         <v>3</v>
       </c>
-      <c r="I16" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="17" ht="17.25" spans="1:9">
+      <c r="I16" s="3">
+        <v>150</v>
+      </c>
+      <c r="J16" s="3">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="17" ht="17.25" spans="1:10">
       <c r="A17" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B17" s="3">
-        <v>86</v>
-      </c>
-      <c r="C17" s="4">
+      <c r="B17" s="4">
+        <v>8600</v>
+      </c>
+      <c r="C17" s="5">
         <v>200</v>
       </c>
-      <c r="D17" s="4">
+      <c r="D17" s="5">
         <v>200</v>
       </c>
-      <c r="E17" s="1">
-        <v>10</v>
-      </c>
-      <c r="F17" s="1">
+      <c r="E17" s="3">
+        <v>10</v>
+      </c>
+      <c r="F17" s="3">
         <v>70</v>
       </c>
       <c r="G17" s="3">
@@ -3333,27 +3513,30 @@
       <c r="H17" s="3">
         <v>3</v>
       </c>
-      <c r="I17" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="18" ht="17.25" spans="1:9">
+      <c r="I17" s="3">
+        <v>150</v>
+      </c>
+      <c r="J17" s="3">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="18" ht="17.25" spans="1:10">
       <c r="A18" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B18" s="3">
-        <v>88</v>
-      </c>
-      <c r="C18" s="4">
+      <c r="B18" s="4">
+        <v>8800</v>
+      </c>
+      <c r="C18" s="5">
         <v>200</v>
       </c>
-      <c r="D18" s="4">
+      <c r="D18" s="5">
         <v>200</v>
       </c>
-      <c r="E18" s="1">
-        <v>10</v>
-      </c>
-      <c r="F18" s="1">
+      <c r="E18" s="3">
+        <v>10</v>
+      </c>
+      <c r="F18" s="3">
         <v>70</v>
       </c>
       <c r="G18" s="3">
@@ -3362,27 +3545,30 @@
       <c r="H18" s="3">
         <v>3</v>
       </c>
-      <c r="I18" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="19" ht="17.25" spans="1:9">
+      <c r="I18" s="3">
+        <v>150</v>
+      </c>
+      <c r="J18" s="3">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="19" ht="17.25" spans="1:10">
       <c r="A19" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B19" s="3">
-        <v>90</v>
-      </c>
-      <c r="C19" s="4">
+      <c r="B19" s="4">
+        <v>9000</v>
+      </c>
+      <c r="C19" s="5">
         <v>500</v>
       </c>
-      <c r="D19" s="4">
+      <c r="D19" s="5">
         <v>500</v>
       </c>
-      <c r="E19" s="1">
-        <v>10</v>
-      </c>
-      <c r="F19" s="1">
+      <c r="E19" s="3">
+        <v>10</v>
+      </c>
+      <c r="F19" s="3">
         <v>70</v>
       </c>
       <c r="G19" s="3">
@@ -3391,27 +3577,30 @@
       <c r="H19" s="3">
         <v>3</v>
       </c>
-      <c r="I19" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="20" ht="17.25" spans="1:9">
+      <c r="I19" s="3">
+        <v>150</v>
+      </c>
+      <c r="J19" s="3">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="20" ht="17.25" spans="1:10">
       <c r="A20" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B20" s="3">
-        <v>92</v>
-      </c>
-      <c r="C20" s="4">
+      <c r="B20" s="4">
+        <v>9200</v>
+      </c>
+      <c r="C20" s="5">
         <v>500</v>
       </c>
-      <c r="D20" s="4">
+      <c r="D20" s="5">
         <v>500</v>
       </c>
-      <c r="E20" s="1">
+      <c r="E20" s="3">
         <v>5</v>
       </c>
-      <c r="F20" s="1">
+      <c r="F20" s="3">
         <v>70</v>
       </c>
       <c r="G20" s="3">
@@ -3420,27 +3609,30 @@
       <c r="H20" s="3">
         <v>2</v>
       </c>
-      <c r="I20" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="21" ht="17.25" spans="1:9">
+      <c r="I20" s="3">
+        <v>150</v>
+      </c>
+      <c r="J20" s="3">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="21" ht="17.25" spans="1:10">
       <c r="A21" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B21" s="3">
-        <v>94</v>
-      </c>
-      <c r="C21" s="4">
+      <c r="B21" s="4">
+        <v>9400</v>
+      </c>
+      <c r="C21" s="5">
         <v>1000</v>
       </c>
-      <c r="D21" s="3">
+      <c r="D21" s="4">
         <v>1000</v>
       </c>
-      <c r="E21" s="1">
+      <c r="E21" s="3">
         <v>5</v>
       </c>
-      <c r="F21" s="1">
+      <c r="F21" s="3">
         <v>70</v>
       </c>
       <c r="G21" s="3">
@@ -3449,27 +3641,30 @@
       <c r="H21" s="3">
         <v>2</v>
       </c>
-      <c r="I21" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="22" ht="17.25" spans="1:9">
+      <c r="I21" s="3">
+        <v>150</v>
+      </c>
+      <c r="J21" s="3">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="22" ht="17.25" spans="1:10">
       <c r="A22" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B22" s="3">
-        <v>96</v>
-      </c>
-      <c r="C22" s="4">
+      <c r="B22" s="4">
+        <v>9600</v>
+      </c>
+      <c r="C22" s="5">
         <v>1000</v>
       </c>
-      <c r="D22" s="3">
+      <c r="D22" s="4">
         <v>1000</v>
       </c>
-      <c r="E22" s="1">
+      <c r="E22" s="3">
         <v>0</v>
       </c>
-      <c r="F22" s="1">
+      <c r="F22" s="3">
         <v>70</v>
       </c>
       <c r="G22" s="3">
@@ -3478,27 +3673,30 @@
       <c r="H22" s="3">
         <v>2</v>
       </c>
-      <c r="I22" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="23" ht="17.25" spans="1:9">
+      <c r="I22" s="3">
+        <v>150</v>
+      </c>
+      <c r="J22" s="3">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="23" ht="17.25" spans="1:10">
       <c r="A23" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B23" s="3">
-        <v>100</v>
-      </c>
-      <c r="C23" s="3">
+      <c r="B23" s="4">
+        <v>10000</v>
+      </c>
+      <c r="C23" s="4">
         <v>9999999</v>
       </c>
-      <c r="D23" s="3">
+      <c r="D23" s="4">
         <v>9999999</v>
       </c>
-      <c r="E23" s="1">
+      <c r="E23" s="3">
         <v>0</v>
       </c>
-      <c r="F23" s="1">
+      <c r="F23" s="3">
         <v>70</v>
       </c>
       <c r="G23" s="3">
@@ -3507,18 +3705,22 @@
       <c r="H23" s="3">
         <v>1</v>
       </c>
-      <c r="I23" s="1" t="s">
-        <v>44</v>
+      <c r="I23" s="3">
+        <v>150</v>
+      </c>
+      <c r="J23" s="3">
+        <v>250</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="7">
-    <mergeCell ref="A1:I1"/>
+  <mergeCells count="8">
+    <mergeCell ref="A1:J1"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="E2:F2"/>
-    <mergeCell ref="G2:I2"/>
+    <mergeCell ref="G2:J2"/>
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="G3:H3"/>
+    <mergeCell ref="I3:J3"/>
     <mergeCell ref="A2:B3"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>